<commit_message>
saving learning states at App
</commit_message>
<xml_diff>
--- a/public/excel/Algorithms.xlsx
+++ b/public/excel/Algorithms.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barte\WebstormProjects\react_stuff\public\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sialalalax\WebstormProjects\untitled\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B464DE24-61BD-4152-9C8C-88F4005C4884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CFF413-0441-4108-AE59-41695EB3E0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="111">
   <si>
     <t>algorithm</t>
   </si>
@@ -111,12 +111,6 @@
     <t>R2 U R' U R' U' R U' R2 U' D R' U R D'</t>
   </si>
   <si>
-    <t>R' U' R U D' R2 U R' U R U' R U' R2 D</t>
-  </si>
-  <si>
-    <t>R U R' U' D R2 U' R U' R' U R' U R2 D'</t>
-  </si>
-  <si>
     <t>R2 F2 R U2 R U2 R' F R U R' U' R' F R2</t>
   </si>
   <si>
@@ -187,6 +181,183 @@
   </si>
   <si>
     <t>OLL</t>
+  </si>
+  <si>
+    <t>U' R' U' R U D' R2 U R' U R U' R U' R2 D</t>
+  </si>
+  <si>
+    <t>U' R U R' U' D R2 U' R U' R' U R' U R2 D'</t>
+  </si>
+  <si>
+    <t>R U2 R2 F R F' U2 R' F R F'</t>
+  </si>
+  <si>
+    <t>r U r' U2 r U2 R' U2 R U' r'</t>
+  </si>
+  <si>
+    <t>l' U2 L U L' U l</t>
+  </si>
+  <si>
+    <t>M U' r U2 r' U' R U' R' M'</t>
+  </si>
+  <si>
+    <t>r U2 R' U' R U' r'</t>
+  </si>
+  <si>
+    <t>r U R' U R U2 r'</t>
+  </si>
+  <si>
+    <t>l' U' L U' L' U2 l</t>
+  </si>
+  <si>
+    <t>R U R' U' R' F R2 U R' U' F'</t>
+  </si>
+  <si>
+    <t>R U R' U R' F R F' R U2 R'</t>
+  </si>
+  <si>
+    <t>r U R' U R' F R F' R U2 r'</t>
+  </si>
+  <si>
+    <t>M' R' U' R U' R' U2 R U' R r'</t>
+  </si>
+  <si>
+    <t>F U R U' R2 F' R U R U' R'</t>
+  </si>
+  <si>
+    <t>R' F R U R' F' R F U' F'</t>
+  </si>
+  <si>
+    <t>l' U' l L' U' L U l' U l</t>
+  </si>
+  <si>
+    <t>r U r' R U R' U' r U' r'</t>
+  </si>
+  <si>
+    <t>r U R' U R U2 r2 U' R U' R' U2 r</t>
+  </si>
+  <si>
+    <t>r' R U R U R' U' M' R' F R F'</t>
+  </si>
+  <si>
+    <t>r U R' U' M2 U R U' R' U' M'</t>
+  </si>
+  <si>
+    <t>R U2 R' U' R U R' U' R U' R'</t>
+  </si>
+  <si>
+    <t>R U2 R2 U' R2 U' R2 U2 R</t>
+  </si>
+  <si>
+    <t>R2 D' R U2 R' D R U2 R</t>
+  </si>
+  <si>
+    <t>r U R' U' r' F R F'</t>
+  </si>
+  <si>
+    <t>F' r U R' U' r' F R</t>
+  </si>
+  <si>
+    <t>R U R' U R U2 R'</t>
+  </si>
+  <si>
+    <t>r U R' U' r' R U R U' R'</t>
+  </si>
+  <si>
+    <t>R U R' U' R U' R' F' U' F R U R'</t>
+  </si>
+  <si>
+    <t>F R' F R2 U' R' U' R U R' F2</t>
+  </si>
+  <si>
+    <t>R' U' F U R U' R' F' R</t>
+  </si>
+  <si>
+    <t>L U F' U' L' U L F L'</t>
+  </si>
+  <si>
+    <t>R U R' U' R' F R F'</t>
+  </si>
+  <si>
+    <t>R U R2 U' R' F R U R U' F'</t>
+  </si>
+  <si>
+    <t>R U2 R2 F R F' R U2 R'</t>
+  </si>
+  <si>
+    <t>L' U' L U' L' U L U L F' L' F</t>
+  </si>
+  <si>
+    <t>F R' F' R U R U' R'</t>
+  </si>
+  <si>
+    <t>R U R' U R U' R' U' R' F R F'</t>
+  </si>
+  <si>
+    <t>L F' L' U' L U F U' L'</t>
+  </si>
+  <si>
+    <t>R' F R U R' U' F' U R</t>
+  </si>
+  <si>
+    <t>R U R' U R U2 R' F R U R' U' F'</t>
+  </si>
+  <si>
+    <t>R' U' R U' R' U2 R F R U R' U' F'</t>
+  </si>
+  <si>
+    <t>F' U' L' U L F</t>
+  </si>
+  <si>
+    <t>F U R U' R' F'</t>
+  </si>
+  <si>
+    <t>F R U R' U' F'</t>
+  </si>
+  <si>
+    <t>R' U' R' F R F' U R</t>
+  </si>
+  <si>
+    <t>R' U' R' F R F' R' F R F' U R</t>
+  </si>
+  <si>
+    <t>F R U R' U' R U R' U' F'</t>
+  </si>
+  <si>
+    <t>r U' r2 U r2 U r2 U' r</t>
+  </si>
+  <si>
+    <t>r' U r2 U' r2 U' r2 U r'</t>
+  </si>
+  <si>
+    <t>F U R U' R' U R U' R' F'</t>
+  </si>
+  <si>
+    <t>R U R' U R U' B U' B' R'</t>
+  </si>
+  <si>
+    <t>l' U2 L U L' U' L U L' U l</t>
+  </si>
+  <si>
+    <t>r U2 R' U' R U R' U' R U' r'</t>
+  </si>
+  <si>
+    <t>R' F R U R U' R2 F' R2 U' R' U R U R'</t>
+  </si>
+  <si>
+    <t>r' U' r U' R' U R U' R' U R r' U r</t>
+  </si>
+  <si>
+    <t>R U R' U' M' U R U' r'</t>
+  </si>
+  <si>
+    <t>R U R' U R' F R F' U2 R' F R F'</t>
+  </si>
+  <si>
+    <t>R' U' R U' R' U2 R</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -222,7 +393,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -271,11 +442,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -292,75 +474,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color auto="1"/>
@@ -694,68 +822,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA72" sqref="AA72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="50.44140625" customWidth="1"/>
-    <col min="3" max="23" width="4.44140625" customWidth="1"/>
-    <col min="24" max="24" width="10.5546875" style="10" customWidth="1"/>
-    <col min="25" max="27" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="3" max="23" width="4.42578125" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" style="9" customWidth="1"/>
+    <col min="25" max="27" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8" t="s">
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8" t="s">
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y1" s="4"/>
+      <c r="Y1" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -825,11 +955,14 @@
       <c r="W2" s="1">
         <v>1</v>
       </c>
-      <c r="X2" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y2" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -899,11 +1032,14 @@
       <c r="W3" s="1">
         <v>1</v>
       </c>
-      <c r="X3" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y3" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -973,11 +1109,14 @@
       <c r="W4" s="1">
         <v>1</v>
       </c>
-      <c r="X4" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y4" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -1047,11 +1186,14 @@
       <c r="W5" s="1">
         <v>1</v>
       </c>
-      <c r="X5" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y5" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1121,16 +1263,19 @@
       <c r="W6" s="1">
         <v>1</v>
       </c>
-      <c r="X6" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y6" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
@@ -1195,16 +1340,19 @@
       <c r="W7" s="1">
         <v>1</v>
       </c>
-      <c r="X7" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y7" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -1269,16 +1417,19 @@
       <c r="W8" s="1">
         <v>1</v>
       </c>
-      <c r="X8" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y8" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -1343,16 +1494,19 @@
       <c r="W9" s="1">
         <v>1</v>
       </c>
-      <c r="X9" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -1417,16 +1571,19 @@
       <c r="W10" s="1">
         <v>1</v>
       </c>
-      <c r="X10" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y10" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
@@ -1491,16 +1648,19 @@
       <c r="W11" s="1">
         <v>1</v>
       </c>
-      <c r="X11" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y11" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -1565,16 +1725,19 @@
       <c r="W12" s="1">
         <v>1</v>
       </c>
-      <c r="X12" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y12" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1">
         <v>4</v>
@@ -1639,16 +1802,19 @@
       <c r="W13" s="1">
         <v>1</v>
       </c>
-      <c r="X13" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y13" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
@@ -1713,16 +1879,19 @@
       <c r="W14" s="1">
         <v>1</v>
       </c>
-      <c r="X14" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y14" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1">
         <v>3</v>
@@ -1787,16 +1956,19 @@
       <c r="W15" s="1">
         <v>1</v>
       </c>
-      <c r="X15" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X15" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y15" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -1861,16 +2033,19 @@
       <c r="W16" s="1">
         <v>1</v>
       </c>
-      <c r="X16" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y16" s="10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
@@ -1935,16 +2110,19 @@
       <c r="W17" s="1">
         <v>1</v>
       </c>
-      <c r="X17" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y17" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
@@ -2009,16 +2187,19 @@
       <c r="W18" s="1">
         <v>1</v>
       </c>
-      <c r="X18" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y18" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
@@ -2083,16 +2264,19 @@
       <c r="W19" s="1">
         <v>1</v>
       </c>
-      <c r="X19" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X19" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y19" s="10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -2157,16 +2341,19 @@
       <c r="W20" s="1">
         <v>1</v>
       </c>
-      <c r="X20" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y20" s="10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1">
         <v>3</v>
@@ -2231,16 +2418,19 @@
       <c r="W21" s="1">
         <v>1</v>
       </c>
-      <c r="X21" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y21" s="10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
@@ -2305,15 +2495,20 @@
       <c r="W22" s="1">
         <v>1</v>
       </c>
-      <c r="X22" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X22" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y22" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>1</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B23" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="C23" s="5">
         <v>0</v>
       </c>
@@ -2377,15 +2572,20 @@
       <c r="W23" s="1">
         <v>0</v>
       </c>
-      <c r="X23" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y23" s="10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>2</v>
       </c>
-      <c r="B24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="C24" s="1">
         <v>0</v>
       </c>
@@ -2449,15 +2649,20 @@
       <c r="W24" s="1">
         <v>0</v>
       </c>
-      <c r="X24" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y24" s="10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>3</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="C25" s="5">
         <v>0</v>
       </c>
@@ -2521,15 +2726,20 @@
       <c r="W25" s="1">
         <v>0</v>
       </c>
-      <c r="X25" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y25" s="10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>4</v>
       </c>
-      <c r="B26" s="7"/>
+      <c r="B26" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
@@ -2593,15 +2803,20 @@
       <c r="W26" s="1">
         <v>1</v>
       </c>
-      <c r="X26" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X26" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y26" s="10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>5</v>
       </c>
-      <c r="B27" s="7"/>
+      <c r="B27" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="C27" s="5">
         <v>0</v>
       </c>
@@ -2665,15 +2880,20 @@
       <c r="W27" s="1">
         <v>0</v>
       </c>
-      <c r="X27" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y27" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>6</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="C28" s="1">
         <v>1</v>
       </c>
@@ -2737,15 +2957,20 @@
       <c r="W28" s="1">
         <v>0</v>
       </c>
-      <c r="X28" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X28" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y28" s="10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>7</v>
       </c>
-      <c r="B29" s="7"/>
+      <c r="B29" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="C29" s="5">
         <v>0</v>
       </c>
@@ -2809,15 +3034,20 @@
       <c r="W29" s="1">
         <v>0</v>
       </c>
-      <c r="X29" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X29" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y29" s="10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>8</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
@@ -2881,15 +3111,20 @@
       <c r="W30" s="1">
         <v>1</v>
       </c>
-      <c r="X30" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X30" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y30" s="10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>9</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="C31" s="5">
         <v>1</v>
       </c>
@@ -2953,15 +3188,20 @@
       <c r="W31" s="1">
         <v>1</v>
       </c>
-      <c r="X31" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X31" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y31" s="10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>10</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="C32" s="1">
         <v>0</v>
       </c>
@@ -3025,15 +3265,20 @@
       <c r="W32" s="1">
         <v>0</v>
       </c>
-      <c r="X32" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X32" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y32" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>11</v>
       </c>
-      <c r="B33" s="7"/>
+      <c r="B33" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="C33" s="5">
         <v>0</v>
       </c>
@@ -3097,15 +3342,20 @@
       <c r="W33" s="1">
         <v>0</v>
       </c>
-      <c r="X33" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X33" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y33" s="10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>12</v>
       </c>
-      <c r="B34" s="7"/>
+      <c r="B34" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="C34" s="1">
         <v>1</v>
       </c>
@@ -3169,15 +3419,20 @@
       <c r="W34" s="1">
         <v>0</v>
       </c>
-      <c r="X34" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X34" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y34" s="10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>13</v>
       </c>
-      <c r="B35" s="7"/>
+      <c r="B35" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="C35" s="5">
         <v>0</v>
       </c>
@@ -3241,15 +3496,20 @@
       <c r="W35" s="1">
         <v>0</v>
       </c>
-      <c r="X35" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X35" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y35" s="10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>14</v>
       </c>
-      <c r="B36" s="7"/>
+      <c r="B36" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="C36" s="1">
         <v>1</v>
       </c>
@@ -3313,15 +3573,20 @@
       <c r="W36" s="1">
         <v>1</v>
       </c>
-      <c r="X36" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X36" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y36" s="10">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>15</v>
       </c>
-      <c r="B37" s="7"/>
+      <c r="B37" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="C37" s="5">
         <v>0</v>
       </c>
@@ -3385,15 +3650,20 @@
       <c r="W37" s="1">
         <v>0</v>
       </c>
-      <c r="X37" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X37" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y37" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>16</v>
       </c>
-      <c r="B38" s="7"/>
+      <c r="B38" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="C38" s="1">
         <v>1</v>
       </c>
@@ -3457,15 +3727,20 @@
       <c r="W38" s="1">
         <v>0</v>
       </c>
-      <c r="X38" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X38" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y38" s="10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>17</v>
       </c>
-      <c r="B39" s="7"/>
+      <c r="B39" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="C39" s="5">
         <v>0</v>
       </c>
@@ -3529,15 +3804,20 @@
       <c r="W39" s="1">
         <v>1</v>
       </c>
-      <c r="X39" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X39" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y39" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>18</v>
       </c>
-      <c r="B40" s="7"/>
+      <c r="B40" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="C40" s="1">
         <v>1</v>
       </c>
@@ -3601,15 +3881,20 @@
       <c r="W40" s="1">
         <v>0</v>
       </c>
-      <c r="X40" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X40" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y40" s="10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>19</v>
       </c>
-      <c r="B41" s="7"/>
+      <c r="B41" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="C41" s="5">
         <v>0</v>
       </c>
@@ -3673,15 +3958,20 @@
       <c r="W41" s="1">
         <v>0</v>
       </c>
-      <c r="X41" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X41" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y41" s="10">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>20</v>
       </c>
-      <c r="B42" s="7"/>
+      <c r="B42" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="C42" s="1">
         <v>0</v>
       </c>
@@ -3745,15 +4035,20 @@
       <c r="W42" s="1">
         <v>1</v>
       </c>
-      <c r="X42" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X42" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y42" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>21</v>
       </c>
-      <c r="B43" s="7"/>
+      <c r="B43" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="C43" s="5">
         <v>1</v>
       </c>
@@ -3817,15 +4112,20 @@
       <c r="W43" s="1">
         <v>0</v>
       </c>
-      <c r="X43" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X43" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y43" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>22</v>
       </c>
-      <c r="B44" s="7"/>
+      <c r="B44" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="C44" s="1">
         <v>0</v>
       </c>
@@ -3889,15 +4189,20 @@
       <c r="W44" s="1">
         <v>0</v>
       </c>
-      <c r="X44" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X44" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y44" s="10">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>23</v>
       </c>
-      <c r="B45" s="7"/>
+      <c r="B45" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="C45" s="5">
         <v>0</v>
       </c>
@@ -3961,15 +4266,20 @@
       <c r="W45" s="1">
         <v>1</v>
       </c>
-      <c r="X45" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X45" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y45" s="10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>24</v>
       </c>
-      <c r="B46" s="7"/>
+      <c r="B46" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="C46" s="1">
         <v>1</v>
       </c>
@@ -4033,15 +4343,20 @@
       <c r="W46" s="1">
         <v>1</v>
       </c>
-      <c r="X46" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X46" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y46" s="10">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>25</v>
       </c>
-      <c r="B47" s="7"/>
+      <c r="B47" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="C47" s="5">
         <v>0</v>
       </c>
@@ -4105,15 +4420,20 @@
       <c r="W47" s="1">
         <v>0</v>
       </c>
-      <c r="X47" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X47" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y47" s="10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>26</v>
       </c>
-      <c r="B48" s="7"/>
+      <c r="B48" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="C48" s="1">
         <v>1</v>
       </c>
@@ -4177,15 +4497,20 @@
       <c r="W48" s="1">
         <v>0</v>
       </c>
-      <c r="X48" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X48" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y48" s="10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>27</v>
       </c>
-      <c r="B49" s="7"/>
+      <c r="B49" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="C49" s="5">
         <v>0</v>
       </c>
@@ -4249,15 +4574,20 @@
       <c r="W49" s="1">
         <v>0</v>
       </c>
-      <c r="X49" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X49" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y49" s="10">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>28</v>
       </c>
-      <c r="B50" s="7"/>
+      <c r="B50" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="C50" s="1">
         <v>0</v>
       </c>
@@ -4321,15 +4651,20 @@
       <c r="W50" s="1">
         <v>1</v>
       </c>
-      <c r="X50" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X50" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y50" s="10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>29</v>
       </c>
-      <c r="B51" s="7"/>
+      <c r="B51" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="C51" s="5">
         <v>1</v>
       </c>
@@ -4393,15 +4728,20 @@
       <c r="W51" s="1">
         <v>1</v>
       </c>
-      <c r="X51" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X51" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y51" s="10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>30</v>
       </c>
-      <c r="B52" s="7"/>
+      <c r="B52" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="C52" s="1">
         <v>0</v>
       </c>
@@ -4465,15 +4805,20 @@
       <c r="W52" s="1">
         <v>1</v>
       </c>
-      <c r="X52" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X52" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y52" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>31</v>
       </c>
-      <c r="B53" s="7"/>
+      <c r="B53" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="C53" s="5">
         <v>1</v>
       </c>
@@ -4537,15 +4882,20 @@
       <c r="W53" s="1">
         <v>1</v>
       </c>
-      <c r="X53" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X53" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y53" s="10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>32</v>
       </c>
-      <c r="B54" s="7"/>
+      <c r="B54" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="C54" s="1">
         <v>0</v>
       </c>
@@ -4609,15 +4959,20 @@
       <c r="W54" s="1">
         <v>0</v>
       </c>
-      <c r="X54" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X54" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y54" s="10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>33</v>
       </c>
-      <c r="B55" s="7"/>
+      <c r="B55" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="C55" s="5">
         <v>1</v>
       </c>
@@ -4681,15 +5036,20 @@
       <c r="W55" s="1">
         <v>1</v>
       </c>
-      <c r="X55" s="9" t="s">
+      <c r="X55" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y55" s="10">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>34</v>
       </c>
-      <c r="B56" s="7"/>
+      <c r="B56" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="C56" s="1">
         <v>0</v>
       </c>
@@ -4753,15 +5113,20 @@
       <c r="W56" s="1">
         <v>1</v>
       </c>
-      <c r="X56" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X56" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y56" s="10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>35</v>
       </c>
-      <c r="B57" s="7"/>
+      <c r="B57" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="C57" s="5">
         <v>1</v>
       </c>
@@ -4825,15 +5190,20 @@
       <c r="W57" s="1">
         <v>1</v>
       </c>
-      <c r="X57" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X57" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y57" s="10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>36</v>
       </c>
-      <c r="B58" s="7"/>
+      <c r="B58" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="C58" s="1">
         <v>0</v>
       </c>
@@ -4897,15 +5267,20 @@
       <c r="W58" s="1">
         <v>1</v>
       </c>
-      <c r="X58" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X58" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y58" s="10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>37</v>
       </c>
-      <c r="B59" s="7"/>
+      <c r="B59" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="C59" s="5">
         <v>1</v>
       </c>
@@ -4969,15 +5344,20 @@
       <c r="W59" s="1">
         <v>1</v>
       </c>
-      <c r="X59" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X59" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y59" s="10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>38</v>
       </c>
-      <c r="B60" s="7"/>
+      <c r="B60" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="C60" s="1">
         <v>0</v>
       </c>
@@ -5041,15 +5421,20 @@
       <c r="W60" s="1">
         <v>0</v>
       </c>
-      <c r="X60" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X60" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y60" s="10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>39</v>
       </c>
-      <c r="B61" s="7"/>
+      <c r="B61" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="C61" s="5">
         <v>0</v>
       </c>
@@ -5113,15 +5498,20 @@
       <c r="W61" s="1">
         <v>0</v>
       </c>
-      <c r="X61" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X61" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y61" s="10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>40</v>
       </c>
-      <c r="B62" s="7"/>
+      <c r="B62" s="7" t="s">
+        <v>90</v>
+      </c>
       <c r="C62" s="1">
         <v>0</v>
       </c>
@@ -5185,15 +5575,20 @@
       <c r="W62" s="1">
         <v>1</v>
       </c>
-      <c r="X62" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X62" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y62" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>41</v>
       </c>
-      <c r="B63" s="7"/>
+      <c r="B63" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="C63" s="5">
         <v>0</v>
       </c>
@@ -5257,15 +5652,20 @@
       <c r="W63" s="1">
         <v>1</v>
       </c>
-      <c r="X63" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X63" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y63" s="10">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>42</v>
       </c>
-      <c r="B64" s="7"/>
+      <c r="B64" s="7" t="s">
+        <v>92</v>
+      </c>
       <c r="C64" s="1">
         <v>1</v>
       </c>
@@ -5329,15 +5729,20 @@
       <c r="W64" s="1">
         <v>0</v>
       </c>
-      <c r="X64" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X64" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y64" s="10">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>43</v>
       </c>
-      <c r="B65" s="7"/>
+      <c r="B65" s="7" t="s">
+        <v>93</v>
+      </c>
       <c r="C65" s="5">
         <v>0</v>
       </c>
@@ -5401,15 +5806,20 @@
       <c r="W65" s="1">
         <v>1</v>
       </c>
-      <c r="X65" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X65" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y65" s="10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>44</v>
       </c>
-      <c r="B66" s="7"/>
+      <c r="B66" s="7" t="s">
+        <v>94</v>
+      </c>
       <c r="C66" s="1">
         <v>0</v>
       </c>
@@ -5473,15 +5883,20 @@
       <c r="W66" s="1">
         <v>0</v>
       </c>
-      <c r="X66" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X66" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y66" s="10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>45</v>
       </c>
-      <c r="B67" s="7"/>
+      <c r="B67" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="C67" s="5">
         <v>0</v>
       </c>
@@ -5545,15 +5960,20 @@
       <c r="W67" s="1">
         <v>1</v>
       </c>
-      <c r="X67" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X67" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y67" s="10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>46</v>
       </c>
-      <c r="B68" s="7"/>
+      <c r="B68" s="7" t="s">
+        <v>96</v>
+      </c>
       <c r="C68" s="1">
         <v>0</v>
       </c>
@@ -5617,15 +6037,20 @@
       <c r="W68" s="1">
         <v>0</v>
       </c>
-      <c r="X68" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X68" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y68" s="10">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>47</v>
       </c>
-      <c r="B69" s="7"/>
+      <c r="B69" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="C69" s="5">
         <v>1</v>
       </c>
@@ -5689,15 +6114,20 @@
       <c r="W69" s="1">
         <v>0</v>
       </c>
-      <c r="X69" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X69" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y69" s="10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>48</v>
       </c>
-      <c r="B70" s="7"/>
+      <c r="B70" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="C70" s="1">
         <v>0</v>
       </c>
@@ -5761,15 +6191,20 @@
       <c r="W70" s="1">
         <v>0</v>
       </c>
-      <c r="X70" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X70" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y70" s="10">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>49</v>
       </c>
-      <c r="B71" s="7"/>
+      <c r="B71" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="C71" s="5">
         <v>0</v>
       </c>
@@ -5833,15 +6268,20 @@
       <c r="W71" s="1">
         <v>0</v>
       </c>
-      <c r="X71" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X71" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y71" s="10">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>50</v>
       </c>
-      <c r="B72" s="7"/>
+      <c r="B72" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="C72" s="1">
         <v>0</v>
       </c>
@@ -5905,15 +6345,20 @@
       <c r="W72" s="1">
         <v>0</v>
       </c>
-      <c r="X72" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X72" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y72" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>51</v>
       </c>
-      <c r="B73" s="7"/>
+      <c r="B73" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="C73" s="5">
         <v>1</v>
       </c>
@@ -5977,15 +6422,20 @@
       <c r="W73" s="1">
         <v>0</v>
       </c>
-      <c r="X73" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X73" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y73" s="10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>52</v>
       </c>
-      <c r="B74" s="7"/>
+      <c r="B74" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="C74" s="1">
         <v>1</v>
       </c>
@@ -6049,15 +6499,20 @@
       <c r="W74" s="1">
         <v>0</v>
       </c>
-      <c r="X74" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X74" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y74" s="10">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>53</v>
       </c>
-      <c r="B75" s="7"/>
+      <c r="B75" s="7" t="s">
+        <v>103</v>
+      </c>
       <c r="C75" s="5">
         <v>1</v>
       </c>
@@ -6121,15 +6576,20 @@
       <c r="W75" s="1">
         <v>0</v>
       </c>
-      <c r="X75" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X75" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y75" s="10">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>54</v>
       </c>
-      <c r="B76" s="7"/>
+      <c r="B76" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="C76" s="1">
         <v>1</v>
       </c>
@@ -6193,15 +6653,20 @@
       <c r="W76" s="1">
         <v>0</v>
       </c>
-      <c r="X76" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X76" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y76" s="10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>55</v>
       </c>
-      <c r="B77" s="7"/>
+      <c r="B77" s="7" t="s">
+        <v>105</v>
+      </c>
       <c r="C77" s="5">
         <v>1</v>
       </c>
@@ -6265,15 +6730,20 @@
       <c r="W77" s="1">
         <v>0</v>
       </c>
-      <c r="X77" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X77" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y77" s="10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>56</v>
       </c>
-      <c r="B78" s="7"/>
+      <c r="B78" s="7" t="s">
+        <v>106</v>
+      </c>
       <c r="C78" s="1">
         <v>0</v>
       </c>
@@ -6337,15 +6807,20 @@
       <c r="W78" s="1">
         <v>0</v>
       </c>
-      <c r="X78" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X78" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y78" s="10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <v>57</v>
       </c>
-      <c r="B79" s="7"/>
+      <c r="B79" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="C79" s="5">
         <v>0</v>
       </c>
@@ -6409,8 +6884,11 @@
       <c r="W79" s="1">
         <v>1</v>
       </c>
-      <c r="X79" s="9" t="s">
-        <v>53</v>
+      <c r="X79" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y79" s="10">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -6423,30 +6901,7 @@
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="O1:Q1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:W22">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23:W79">
+  <conditionalFormatting sqref="C2:W79">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>5</formula>
     </cfRule>

</xml_diff>

<commit_message>
saving algorithms training results
</commit_message>
<xml_diff>
--- a/public/excel/Algorithms.xlsx
+++ b/public/excel/Algorithms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sialalalax\WebstormProjects\untitled\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CFF413-0441-4108-AE59-41695EB3E0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADDC7BA-8A7F-4C03-ABC8-0A096D84EF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,7 +393,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -442,22 +442,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -480,7 +469,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -823,7 +811,7 @@
   <dimension ref="A1:AA79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA72" sqref="AA72"/>
+      <selection activeCell="AB18" sqref="AB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,41 +829,41 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11" t="s">
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11" t="s">
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11" t="s">
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11" t="s">
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
       <c r="X1" s="2" t="s">
         <v>49</v>
       </c>
@@ -958,7 +946,7 @@
       <c r="X2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="10">
+      <c r="Y2" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1035,7 +1023,7 @@
       <c r="X3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y3" s="10">
+      <c r="Y3" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1112,7 +1100,7 @@
       <c r="X4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y4" s="10">
+      <c r="Y4" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1189,7 +1177,7 @@
       <c r="X5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y5" s="10">
+      <c r="Y5" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1266,7 +1254,7 @@
       <c r="X6" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y6" s="10">
+      <c r="Y6" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1343,7 +1331,7 @@
       <c r="X7" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y7" s="10">
+      <c r="Y7" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1420,7 +1408,7 @@
       <c r="X8" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y8" s="10">
+      <c r="Y8" s="1">
         <v>6</v>
       </c>
     </row>
@@ -1497,7 +1485,7 @@
       <c r="X9" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y9" s="10">
+      <c r="Y9" s="1">
         <v>7</v>
       </c>
     </row>
@@ -1574,7 +1562,7 @@
       <c r="X10" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y10" s="10">
+      <c r="Y10" s="1">
         <v>8</v>
       </c>
     </row>
@@ -1651,7 +1639,7 @@
       <c r="X11" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y11" s="10">
+      <c r="Y11" s="1">
         <v>9</v>
       </c>
     </row>
@@ -1728,7 +1716,7 @@
       <c r="X12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y12" s="10">
+      <c r="Y12" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1805,7 +1793,7 @@
       <c r="X13" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y13" s="10">
+      <c r="Y13" s="1">
         <v>11</v>
       </c>
     </row>
@@ -1882,7 +1870,7 @@
       <c r="X14" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y14" s="10">
+      <c r="Y14" s="1">
         <v>12</v>
       </c>
     </row>
@@ -1959,7 +1947,7 @@
       <c r="X15" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y15" s="10">
+      <c r="Y15" s="1">
         <v>13</v>
       </c>
     </row>
@@ -2036,7 +2024,7 @@
       <c r="X16" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y16" s="10">
+      <c r="Y16" s="1">
         <v>14</v>
       </c>
     </row>
@@ -2113,7 +2101,7 @@
       <c r="X17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y17" s="10">
+      <c r="Y17" s="1">
         <v>15</v>
       </c>
     </row>
@@ -2190,7 +2178,7 @@
       <c r="X18" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y18" s="10">
+      <c r="Y18" s="1">
         <v>16</v>
       </c>
     </row>
@@ -2267,7 +2255,7 @@
       <c r="X19" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y19" s="10">
+      <c r="Y19" s="1">
         <v>17</v>
       </c>
     </row>
@@ -2344,7 +2332,7 @@
       <c r="X20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y20" s="10">
+      <c r="Y20" s="1">
         <v>18</v>
       </c>
     </row>
@@ -2421,7 +2409,7 @@
       <c r="X21" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y21" s="10">
+      <c r="Y21" s="1">
         <v>19</v>
       </c>
     </row>
@@ -2498,7 +2486,7 @@
       <c r="X22" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y22" s="10">
+      <c r="Y22" s="1">
         <v>20</v>
       </c>
     </row>
@@ -2575,7 +2563,7 @@
       <c r="X23" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y23" s="10">
+      <c r="Y23" s="1">
         <v>21</v>
       </c>
     </row>
@@ -2652,7 +2640,7 @@
       <c r="X24" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y24" s="10">
+      <c r="Y24" s="1">
         <v>22</v>
       </c>
     </row>
@@ -2729,7 +2717,7 @@
       <c r="X25" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y25" s="10">
+      <c r="Y25" s="1">
         <v>23</v>
       </c>
     </row>
@@ -2806,7 +2794,7 @@
       <c r="X26" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y26" s="10">
+      <c r="Y26" s="1">
         <v>24</v>
       </c>
     </row>
@@ -2883,7 +2871,7 @@
       <c r="X27" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y27" s="10">
+      <c r="Y27" s="1">
         <v>25</v>
       </c>
     </row>
@@ -2960,7 +2948,7 @@
       <c r="X28" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y28" s="10">
+      <c r="Y28" s="1">
         <v>26</v>
       </c>
     </row>
@@ -3037,7 +3025,7 @@
       <c r="X29" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y29" s="10">
+      <c r="Y29" s="1">
         <v>27</v>
       </c>
     </row>
@@ -3114,7 +3102,7 @@
       <c r="X30" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y30" s="10">
+      <c r="Y30" s="1">
         <v>28</v>
       </c>
     </row>
@@ -3191,7 +3179,7 @@
       <c r="X31" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y31" s="10">
+      <c r="Y31" s="1">
         <v>29</v>
       </c>
     </row>
@@ -3268,7 +3256,7 @@
       <c r="X32" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y32" s="10">
+      <c r="Y32" s="1">
         <v>30</v>
       </c>
     </row>
@@ -3345,7 +3333,7 @@
       <c r="X33" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y33" s="10">
+      <c r="Y33" s="1">
         <v>31</v>
       </c>
     </row>
@@ -3422,7 +3410,7 @@
       <c r="X34" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y34" s="10">
+      <c r="Y34" s="1">
         <v>32</v>
       </c>
     </row>
@@ -3499,7 +3487,7 @@
       <c r="X35" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y35" s="10">
+      <c r="Y35" s="1">
         <v>33</v>
       </c>
     </row>
@@ -3576,7 +3564,7 @@
       <c r="X36" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y36" s="10">
+      <c r="Y36" s="1">
         <v>34</v>
       </c>
     </row>
@@ -3653,7 +3641,7 @@
       <c r="X37" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y37" s="10">
+      <c r="Y37" s="1">
         <v>35</v>
       </c>
     </row>
@@ -3730,7 +3718,7 @@
       <c r="X38" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y38" s="10">
+      <c r="Y38" s="1">
         <v>36</v>
       </c>
     </row>
@@ -3807,7 +3795,7 @@
       <c r="X39" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y39" s="10">
+      <c r="Y39" s="1">
         <v>37</v>
       </c>
     </row>
@@ -3884,7 +3872,7 @@
       <c r="X40" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y40" s="10">
+      <c r="Y40" s="1">
         <v>38</v>
       </c>
     </row>
@@ -3961,7 +3949,7 @@
       <c r="X41" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y41" s="10">
+      <c r="Y41" s="1">
         <v>39</v>
       </c>
     </row>
@@ -4038,7 +4026,7 @@
       <c r="X42" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y42" s="10">
+      <c r="Y42" s="1">
         <v>40</v>
       </c>
     </row>
@@ -4115,7 +4103,7 @@
       <c r="X43" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y43" s="10">
+      <c r="Y43" s="1">
         <v>41</v>
       </c>
     </row>
@@ -4192,7 +4180,7 @@
       <c r="X44" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y44" s="10">
+      <c r="Y44" s="1">
         <v>42</v>
       </c>
     </row>
@@ -4269,7 +4257,7 @@
       <c r="X45" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y45" s="10">
+      <c r="Y45" s="1">
         <v>43</v>
       </c>
     </row>
@@ -4346,7 +4334,7 @@
       <c r="X46" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y46" s="10">
+      <c r="Y46" s="1">
         <v>44</v>
       </c>
     </row>
@@ -4423,7 +4411,7 @@
       <c r="X47" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y47" s="10">
+      <c r="Y47" s="1">
         <v>45</v>
       </c>
     </row>
@@ -4500,7 +4488,7 @@
       <c r="X48" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y48" s="10">
+      <c r="Y48" s="1">
         <v>46</v>
       </c>
     </row>
@@ -4577,7 +4565,7 @@
       <c r="X49" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y49" s="10">
+      <c r="Y49" s="1">
         <v>47</v>
       </c>
     </row>
@@ -4654,7 +4642,7 @@
       <c r="X50" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y50" s="10">
+      <c r="Y50" s="1">
         <v>48</v>
       </c>
     </row>
@@ -4731,7 +4719,7 @@
       <c r="X51" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y51" s="10">
+      <c r="Y51" s="1">
         <v>49</v>
       </c>
     </row>
@@ -4808,7 +4796,7 @@
       <c r="X52" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y52" s="10">
+      <c r="Y52" s="1">
         <v>50</v>
       </c>
     </row>
@@ -4885,7 +4873,7 @@
       <c r="X53" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y53" s="10">
+      <c r="Y53" s="1">
         <v>51</v>
       </c>
     </row>
@@ -4962,7 +4950,7 @@
       <c r="X54" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y54" s="10">
+      <c r="Y54" s="1">
         <v>52</v>
       </c>
     </row>
@@ -5039,7 +5027,7 @@
       <c r="X55" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y55" s="10">
+      <c r="Y55" s="1">
         <v>53</v>
       </c>
     </row>
@@ -5116,7 +5104,7 @@
       <c r="X56" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y56" s="10">
+      <c r="Y56" s="1">
         <v>54</v>
       </c>
     </row>
@@ -5193,7 +5181,7 @@
       <c r="X57" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y57" s="10">
+      <c r="Y57" s="1">
         <v>55</v>
       </c>
     </row>
@@ -5270,7 +5258,7 @@
       <c r="X58" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y58" s="10">
+      <c r="Y58" s="1">
         <v>56</v>
       </c>
     </row>
@@ -5347,7 +5335,7 @@
       <c r="X59" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y59" s="10">
+      <c r="Y59" s="1">
         <v>57</v>
       </c>
     </row>
@@ -5424,7 +5412,7 @@
       <c r="X60" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y60" s="10">
+      <c r="Y60" s="1">
         <v>58</v>
       </c>
     </row>
@@ -5501,7 +5489,7 @@
       <c r="X61" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y61" s="10">
+      <c r="Y61" s="1">
         <v>59</v>
       </c>
     </row>
@@ -5578,7 +5566,7 @@
       <c r="X62" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y62" s="10">
+      <c r="Y62" s="1">
         <v>60</v>
       </c>
     </row>
@@ -5655,7 +5643,7 @@
       <c r="X63" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y63" s="10">
+      <c r="Y63" s="1">
         <v>61</v>
       </c>
     </row>
@@ -5732,7 +5720,7 @@
       <c r="X64" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y64" s="10">
+      <c r="Y64" s="1">
         <v>62</v>
       </c>
     </row>
@@ -5809,7 +5797,7 @@
       <c r="X65" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y65" s="10">
+      <c r="Y65" s="1">
         <v>63</v>
       </c>
     </row>
@@ -5886,7 +5874,7 @@
       <c r="X66" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y66" s="10">
+      <c r="Y66" s="1">
         <v>64</v>
       </c>
     </row>
@@ -5963,7 +5951,7 @@
       <c r="X67" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y67" s="10">
+      <c r="Y67" s="1">
         <v>65</v>
       </c>
     </row>
@@ -6040,7 +6028,7 @@
       <c r="X68" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y68" s="10">
+      <c r="Y68" s="1">
         <v>66</v>
       </c>
     </row>
@@ -6117,7 +6105,7 @@
       <c r="X69" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y69" s="10">
+      <c r="Y69" s="1">
         <v>67</v>
       </c>
     </row>
@@ -6194,7 +6182,7 @@
       <c r="X70" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y70" s="10">
+      <c r="Y70" s="1">
         <v>68</v>
       </c>
     </row>
@@ -6271,7 +6259,7 @@
       <c r="X71" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y71" s="10">
+      <c r="Y71" s="1">
         <v>69</v>
       </c>
     </row>
@@ -6348,7 +6336,7 @@
       <c r="X72" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y72" s="10">
+      <c r="Y72" s="1">
         <v>70</v>
       </c>
     </row>
@@ -6425,7 +6413,7 @@
       <c r="X73" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y73" s="10">
+      <c r="Y73" s="1">
         <v>71</v>
       </c>
     </row>
@@ -6502,7 +6490,7 @@
       <c r="X74" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y74" s="10">
+      <c r="Y74" s="1">
         <v>72</v>
       </c>
     </row>
@@ -6579,7 +6567,7 @@
       <c r="X75" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y75" s="10">
+      <c r="Y75" s="1">
         <v>73</v>
       </c>
     </row>
@@ -6656,7 +6644,7 @@
       <c r="X76" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y76" s="10">
+      <c r="Y76" s="1">
         <v>74</v>
       </c>
     </row>
@@ -6733,7 +6721,7 @@
       <c r="X77" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y77" s="10">
+      <c r="Y77" s="1">
         <v>75</v>
       </c>
     </row>
@@ -6810,7 +6798,7 @@
       <c r="X78" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y78" s="10">
+      <c r="Y78" s="1">
         <v>76</v>
       </c>
     </row>
@@ -6887,7 +6875,7 @@
       <c r="X79" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="Y79" s="10">
+      <c r="Y79" s="1">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replacing rotations and wide moves, deleting results for algorithms, fixed stats
</commit_message>
<xml_diff>
--- a/public/excel/Algorithms.xlsx
+++ b/public/excel/Algorithms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sialalalax\WebstormProjects\untitled\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C03904-6C9F-413A-93FE-A2EFDF5B8CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7CAE56-C09D-4EDA-A99F-2948C203F0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="780" windowWidth="28350" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -470,172 +470,7 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color auto="1"/>
@@ -970,7 +805,7 @@
   <dimension ref="A1:AA79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC71" sqref="AC71"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7048,49 +6883,26 @@
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="O1:Q1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:W22">
-    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
+  <conditionalFormatting sqref="C2:W79">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="14" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23:W79">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixed scrambling for algorithms
</commit_message>
<xml_diff>
--- a/public/excel/Algorithms.xlsx
+++ b/public/excel/Algorithms.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barte\WebstormProjects\react_stuff\public\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sialalalax\WebstormProjects\untitled\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116CD3AF-D5BD-4857-BCD8-FBB94C300B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F9DCB4-29D0-4B59-BAD4-9ADB9760E02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arkusz1!$A$1:$Y$79</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="112">
   <si>
     <t>algorithm</t>
   </si>
@@ -358,6 +361,9 @@
   </si>
   <si>
     <t>y' R U R' U' D R2 U' R U' R' U R' U R2 D'</t>
+  </si>
+  <si>
+    <t>r' R2 U R' U r U2 r' U M'</t>
   </si>
 </sst>
 </file>
@@ -804,19 +810,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="50.44140625" customWidth="1"/>
-    <col min="3" max="23" width="4.44140625" customWidth="1"/>
-    <col min="24" max="24" width="7.109375" customWidth="1"/>
-    <col min="25" max="27" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="3" max="23" width="4.42578125" customWidth="1"/>
+    <col min="24" max="24" width="7.140625" customWidth="1"/>
+    <col min="25" max="27" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -867,7 +873,7 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -944,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1329,7 +1335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1406,7 +1412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -1560,7 +1566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1791,7 +1797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -1868,7 +1874,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -1945,7 +1951,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
@@ -2022,7 +2028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -2099,7 +2105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
@@ -2176,7 +2182,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
@@ -2253,7 +2259,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -2330,7 +2336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
@@ -2407,7 +2413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -2484,7 +2490,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>1</v>
       </c>
@@ -2561,7 +2567,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>2</v>
       </c>
@@ -2638,12 +2644,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>3</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
@@ -2715,7 +2721,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>4</v>
       </c>
@@ -2792,7 +2798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>5</v>
       </c>
@@ -2869,7 +2875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>6</v>
       </c>
@@ -2946,7 +2952,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>7</v>
       </c>
@@ -3023,7 +3029,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>8</v>
       </c>
@@ -3100,7 +3106,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>9</v>
       </c>
@@ -3177,7 +3183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>10</v>
       </c>
@@ -3254,7 +3260,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>11</v>
       </c>
@@ -3331,7 +3337,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>12</v>
       </c>
@@ -3408,7 +3414,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>13</v>
       </c>
@@ -3485,7 +3491,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>14</v>
       </c>
@@ -3562,7 +3568,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>15</v>
       </c>
@@ -3639,7 +3645,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>16</v>
       </c>
@@ -3716,7 +3722,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>17</v>
       </c>
@@ -3793,7 +3799,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>18</v>
       </c>
@@ -3870,7 +3876,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>19</v>
       </c>
@@ -3947,7 +3953,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>20</v>
       </c>
@@ -4024,7 +4030,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>21</v>
       </c>
@@ -4101,7 +4107,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>22</v>
       </c>
@@ -4178,7 +4184,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>23</v>
       </c>
@@ -4255,7 +4261,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>24</v>
       </c>
@@ -4332,7 +4338,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>25</v>
       </c>
@@ -4409,7 +4415,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>26</v>
       </c>
@@ -4486,7 +4492,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>27</v>
       </c>
@@ -4563,7 +4569,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>28</v>
       </c>
@@ -4640,7 +4646,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>29</v>
       </c>
@@ -4717,7 +4723,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>30</v>
       </c>
@@ -4794,7 +4800,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>31</v>
       </c>
@@ -4871,7 +4877,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>32</v>
       </c>
@@ -4948,7 +4954,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>33</v>
       </c>
@@ -5025,7 +5031,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>34</v>
       </c>
@@ -5102,7 +5108,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>35</v>
       </c>
@@ -5179,7 +5185,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>36</v>
       </c>
@@ -5256,7 +5262,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>37</v>
       </c>
@@ -5333,7 +5339,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>38</v>
       </c>
@@ -5410,7 +5416,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>39</v>
       </c>
@@ -5487,7 +5493,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>40</v>
       </c>
@@ -5564,7 +5570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>41</v>
       </c>
@@ -5641,7 +5647,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>42</v>
       </c>
@@ -5718,7 +5724,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>43</v>
       </c>
@@ -5795,7 +5801,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>44</v>
       </c>
@@ -5872,7 +5878,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>45</v>
       </c>
@@ -5949,7 +5955,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>46</v>
       </c>
@@ -6026,7 +6032,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>47</v>
       </c>
@@ -6103,7 +6109,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>48</v>
       </c>
@@ -6180,7 +6186,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>49</v>
       </c>
@@ -6257,7 +6263,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>50</v>
       </c>
@@ -6334,7 +6340,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>51</v>
       </c>
@@ -6411,7 +6417,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>52</v>
       </c>
@@ -6488,7 +6494,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>53</v>
       </c>
@@ -6565,7 +6571,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>54</v>
       </c>
@@ -6642,7 +6648,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>55</v>
       </c>
@@ -6719,7 +6725,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>56</v>
       </c>
@@ -6796,7 +6802,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <v>57</v>
       </c>
@@ -6874,6 +6880,22 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Y79" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2" showButton="0"/>
+    <filterColumn colId="3" showButton="0"/>
+    <filterColumn colId="5" showButton="0"/>
+    <filterColumn colId="6" showButton="0"/>
+    <filterColumn colId="8" showButton="0"/>
+    <filterColumn colId="9" showButton="0"/>
+    <filterColumn colId="11" showButton="0"/>
+    <filterColumn colId="12" showButton="0"/>
+    <filterColumn colId="14" showButton="0"/>
+    <filterColumn colId="15" showButton="0"/>
+    <filterColumn colId="17" showButton="0"/>
+    <filterColumn colId="18" showButton="0"/>
+    <filterColumn colId="20" showButton="0"/>
+    <filterColumn colId="21" showButton="0"/>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="R1:T1"/>
     <mergeCell ref="U1:W1"/>

</xml_diff>

<commit_message>
some small changes, saving algorithms tab
</commit_message>
<xml_diff>
--- a/public/excel/Algorithms.xlsx
+++ b/public/excel/Algorithms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sialalalax\WebstormProjects\untitled\public\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barte\WebstormProjects\react_stuff\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F9DCB4-29D0-4B59-BAD4-9ADB9760E02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9E5A29-959F-4359-A013-B6C77FAB937B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -810,19 +810,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
-    <col min="3" max="23" width="4.42578125" customWidth="1"/>
-    <col min="24" max="24" width="7.140625" customWidth="1"/>
-    <col min="25" max="27" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="50.44140625" customWidth="1"/>
+    <col min="3" max="23" width="4.44140625" customWidth="1"/>
+    <col min="24" max="24" width="7.109375" customWidth="1"/>
+    <col min="25" max="27" width="6.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -873,7 +873,7 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -950,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>1</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>2</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>3</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>4</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>5</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>6</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>7</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>8</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>9</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>10</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>11</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>12</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>13</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>14</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>15</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>16</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>17</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>18</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>19</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>20</v>
       </c>
@@ -4030,7 +4030,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>21</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>22</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>23</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>24</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>25</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>26</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>27</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>28</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>29</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>30</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>31</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>32</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>33</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>34</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>35</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>36</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>37</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>38</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>39</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>40</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>41</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>42</v>
       </c>
@@ -5724,7 +5724,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>43</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>44</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>45</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>46</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>47</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>48</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>49</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>50</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>51</v>
       </c>
@@ -6417,7 +6417,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>52</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <v>53</v>
       </c>
@@ -6571,7 +6571,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <v>54</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
         <v>55</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
         <v>56</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
         <v>57</v>
       </c>

</xml_diff>